<commit_message>
added ERD and updated risk assess
</commit_message>
<xml_diff>
--- a/RiskAssessment.xlsx
+++ b/RiskAssessment.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aaa\Documents\QA\SFIAProject-1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\SFIAProject-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{33F59EC6-4980-4CFF-90C9-A644CB5CEA18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23235" yWindow="1080" windowWidth="21600" windowHeight="11835" xr2:uid="{147B9712-7372-45E1-8EF7-258EE806F80D}"/>
+    <workbookView xWindow="-23235" yWindow="1080" windowWidth="21600" windowHeight="11835"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
   <si>
     <t>Description</t>
   </si>
@@ -105,12 +104,6 @@
     <t>website may go dark</t>
   </si>
   <si>
-    <t>Unauthorized people may gain access to the website and view private information</t>
-  </si>
-  <si>
-    <t>A hacker may try to gain access to the databse</t>
-  </si>
-  <si>
     <t>A worker who may not be experienced might accidentally delete some data</t>
   </si>
   <si>
@@ -126,16 +119,25 @@
     <t>Ensures only authorized people have access to the database</t>
   </si>
   <si>
-    <t>Keeps an eye for any attackers trying to gain access to the webapp</t>
-  </si>
-  <si>
     <t>Only Trustworthy and experienced people will be able to delete data</t>
+  </si>
+  <si>
+    <t>The app will be hosted on the cloud so therefore the cloud provider is responsible for the upkeep of the website</t>
+  </si>
+  <si>
+    <t>Unauthorized people may gain access to the website and view private information alter the data</t>
+  </si>
+  <si>
+    <t>A hacker may try to gain access to the databse to steal information</t>
+  </si>
+  <si>
+    <t>Keeps an eye for any attackers trying to gain access to the webapp and act accordingly</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -486,21 +488,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DB0FCC6-C788-4880-9222-8FB72CE0259C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.7109375" customWidth="1"/>
     <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
@@ -535,12 +538,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="2:11" s="1" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>15</v>
@@ -561,18 +564,18 @@
         <v>19</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="2:11" s="1" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
@@ -593,18 +596,18 @@
         <v>20</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="2:11" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>15</v>
@@ -625,7 +628,7 @@
         <v>21</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>22</v>
@@ -636,7 +639,7 @@
         <v>23</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>15</v>
@@ -648,7 +651,7 @@
         <v>16</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>18</v>
@@ -656,8 +659,11 @@
       <c r="I7" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="J7" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="K7" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>